<commit_message>
fix: update m thread
</commit_message>
<xml_diff>
--- a/excel/m_thread.xlsx
+++ b/excel/m_thread.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\FLUTTER\project\MY_GITHUB\thread_fon\thread_fon_db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E9499F-5F03-4AF7-ABEC-912EA7A7349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E67CF4-AE05-483C-9D4A-F49F4E6B31BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{065E2E10-44EF-4F04-9A81-3EF8E78F7D6E}"/>
+    <workbookView xWindow="-52920" yWindow="3495" windowWidth="24240" windowHeight="13740" xr2:uid="{065E2E10-44EF-4F04-9A81-3EF8E78F7D6E}"/>
   </bookViews>
   <sheets>
     <sheet name="m_tolerance" sheetId="4" r:id="rId1"/>
@@ -513,7 +513,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,42 +521,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -565,41 +550,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+      <border outline="0">
+        <top style="thin">
           <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -607,13 +568,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -630,7 +584,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F225511-288B-41EE-ABD9-6B22750955EE}" name="Таблица3" displayName="Таблица3" ref="A1:EN69" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F225511-288B-41EE-ABD9-6B22750955EE}" name="Таблица3" displayName="Таблица3" ref="A1:EN69" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:EN69" xr:uid="{2F225511-288B-41EE-ABD9-6B22750955EE}"/>
   <tableColumns count="144">
     <tableColumn id="1" xr3:uid="{EA54CBA2-69D3-4000-8AF3-24224513245F}" name="id"/>
@@ -1115,585 +1069,585 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3E1EE5-36CA-4568-AA50-5AD4E0DC26A6}">
   <dimension ref="A1:EN69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="CI5" sqref="CI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" customWidth="1"/>
-    <col min="23" max="23" width="15.42578125" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" customWidth="1"/>
-    <col min="25" max="25" width="14.85546875" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1"/>
-    <col min="28" max="28" width="15.42578125" customWidth="1"/>
-    <col min="29" max="29" width="15.85546875" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" customWidth="1"/>
-    <col min="34" max="34" width="15.85546875" customWidth="1"/>
-    <col min="35" max="35" width="12.7109375" customWidth="1"/>
-    <col min="36" max="36" width="12.42578125" customWidth="1"/>
-    <col min="37" max="37" width="13.7109375" customWidth="1"/>
-    <col min="38" max="38" width="13.42578125" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" customWidth="1"/>
-    <col min="41" max="41" width="12.42578125" customWidth="1"/>
-    <col min="42" max="42" width="13.7109375" customWidth="1"/>
-    <col min="43" max="43" width="13.42578125" customWidth="1"/>
-    <col min="44" max="44" width="13.7109375" customWidth="1"/>
-    <col min="45" max="45" width="12.42578125" customWidth="1"/>
-    <col min="46" max="46" width="12.140625" customWidth="1"/>
-    <col min="47" max="47" width="13.42578125" customWidth="1"/>
-    <col min="48" max="48" width="13.140625" customWidth="1"/>
-    <col min="49" max="49" width="13.42578125" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" customWidth="1"/>
-    <col min="51" max="51" width="12.42578125" customWidth="1"/>
-    <col min="52" max="52" width="13.7109375" customWidth="1"/>
-    <col min="53" max="53" width="13.42578125" customWidth="1"/>
-    <col min="54" max="54" width="13.7109375" customWidth="1"/>
-    <col min="55" max="55" width="12.7109375" customWidth="1"/>
-    <col min="56" max="56" width="12.42578125" customWidth="1"/>
-    <col min="57" max="57" width="13.7109375" customWidth="1"/>
-    <col min="58" max="58" width="13.42578125" customWidth="1"/>
-    <col min="59" max="59" width="13.7109375" customWidth="1"/>
-    <col min="60" max="60" width="14.85546875" customWidth="1"/>
-    <col min="61" max="61" width="14.42578125" customWidth="1"/>
-    <col min="62" max="62" width="15.85546875" customWidth="1"/>
-    <col min="63" max="63" width="15.42578125" customWidth="1"/>
-    <col min="64" max="64" width="15.85546875" customWidth="1"/>
-    <col min="65" max="65" width="14.85546875" customWidth="1"/>
-    <col min="66" max="66" width="14.42578125" customWidth="1"/>
-    <col min="67" max="67" width="15.85546875" customWidth="1"/>
-    <col min="68" max="68" width="15.42578125" customWidth="1"/>
-    <col min="69" max="69" width="15.85546875" customWidth="1"/>
-    <col min="70" max="70" width="14.85546875" customWidth="1"/>
-    <col min="71" max="71" width="14.42578125" customWidth="1"/>
-    <col min="72" max="72" width="15.85546875" customWidth="1"/>
-    <col min="73" max="73" width="15.42578125" customWidth="1"/>
-    <col min="74" max="74" width="15.85546875" customWidth="1"/>
-    <col min="75" max="75" width="12.7109375" customWidth="1"/>
-    <col min="76" max="76" width="12.42578125" customWidth="1"/>
-    <col min="77" max="77" width="13.7109375" customWidth="1"/>
-    <col min="78" max="79" width="13.42578125" customWidth="1"/>
-    <col min="80" max="80" width="12.7109375" customWidth="1"/>
-    <col min="81" max="81" width="12.42578125" customWidth="1"/>
-    <col min="82" max="82" width="13.7109375" customWidth="1"/>
-    <col min="83" max="84" width="13.42578125" customWidth="1"/>
-    <col min="85" max="85" width="14.85546875" customWidth="1"/>
-    <col min="86" max="86" width="14.42578125" customWidth="1"/>
-    <col min="87" max="87" width="15.85546875" customWidth="1"/>
-    <col min="88" max="89" width="15.42578125" customWidth="1"/>
-    <col min="90" max="90" width="14.85546875" customWidth="1"/>
-    <col min="91" max="91" width="14.42578125" customWidth="1"/>
-    <col min="92" max="92" width="15.85546875" customWidth="1"/>
-    <col min="93" max="94" width="15.42578125" customWidth="1"/>
-    <col min="95" max="95" width="11.42578125" customWidth="1"/>
-    <col min="96" max="96" width="12.7109375" customWidth="1"/>
-    <col min="97" max="97" width="12.42578125" customWidth="1"/>
-    <col min="98" max="98" width="12.7109375" customWidth="1"/>
-    <col min="99" max="99" width="12.42578125" customWidth="1"/>
-    <col min="100" max="100" width="13.42578125" customWidth="1"/>
-    <col min="101" max="101" width="14.85546875" customWidth="1"/>
-    <col min="102" max="102" width="14.42578125" customWidth="1"/>
-    <col min="103" max="103" width="14.85546875" customWidth="1"/>
-    <col min="104" max="104" width="14.42578125" customWidth="1"/>
-    <col min="105" max="105" width="11.42578125" customWidth="1"/>
-    <col min="106" max="106" width="12.7109375" customWidth="1"/>
-    <col min="107" max="107" width="12.42578125" customWidth="1"/>
-    <col min="108" max="108" width="12.7109375" customWidth="1"/>
-    <col min="109" max="109" width="12.42578125" customWidth="1"/>
-    <col min="110" max="110" width="11.42578125" customWidth="1"/>
-    <col min="111" max="111" width="12.7109375" customWidth="1"/>
-    <col min="112" max="112" width="12.42578125" customWidth="1"/>
-    <col min="113" max="113" width="12.7109375" customWidth="1"/>
-    <col min="114" max="114" width="12.42578125" customWidth="1"/>
-    <col min="115" max="115" width="11.42578125" customWidth="1"/>
-    <col min="116" max="116" width="12.7109375" customWidth="1"/>
-    <col min="117" max="117" width="12.42578125" customWidth="1"/>
-    <col min="118" max="118" width="12.7109375" customWidth="1"/>
-    <col min="119" max="119" width="12.42578125" customWidth="1"/>
-    <col min="120" max="120" width="11.42578125" customWidth="1"/>
-    <col min="121" max="121" width="12.7109375" customWidth="1"/>
-    <col min="122" max="122" width="12.42578125" customWidth="1"/>
-    <col min="123" max="123" width="12.7109375" customWidth="1"/>
-    <col min="124" max="124" width="12.42578125" customWidth="1"/>
-    <col min="125" max="125" width="11.42578125" customWidth="1"/>
-    <col min="126" max="126" width="12.7109375" customWidth="1"/>
-    <col min="127" max="127" width="12.42578125" customWidth="1"/>
-    <col min="128" max="128" width="12.7109375" customWidth="1"/>
-    <col min="129" max="129" width="12.42578125" customWidth="1"/>
-    <col min="130" max="130" width="11.42578125" customWidth="1"/>
-    <col min="131" max="131" width="12.7109375" customWidth="1"/>
-    <col min="132" max="132" width="12.42578125" customWidth="1"/>
-    <col min="133" max="133" width="12.7109375" customWidth="1"/>
-    <col min="134" max="134" width="12.42578125" customWidth="1"/>
-    <col min="135" max="135" width="11.42578125" customWidth="1"/>
-    <col min="136" max="136" width="12.7109375" customWidth="1"/>
-    <col min="137" max="137" width="12.42578125" customWidth="1"/>
-    <col min="138" max="138" width="12.7109375" customWidth="1"/>
-    <col min="139" max="139" width="12.42578125" customWidth="1"/>
-    <col min="140" max="140" width="11.42578125" customWidth="1"/>
-    <col min="141" max="141" width="12.7109375" customWidth="1"/>
-    <col min="142" max="142" width="12.42578125" customWidth="1"/>
-    <col min="143" max="143" width="12.7109375" customWidth="1"/>
-    <col min="144" max="144" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="84" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="88" max="89" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" t="s">
         <v>44</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" t="s">
         <v>45</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" t="s">
         <v>46</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" t="s">
         <v>47</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" t="s">
         <v>48</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" t="s">
         <v>49</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" t="s">
         <v>50</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" t="s">
         <v>51</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" t="s">
         <v>52</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" t="s">
         <v>54</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" t="s">
         <v>55</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" t="s">
         <v>56</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" t="s">
         <v>57</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" t="s">
         <v>58</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" t="s">
         <v>59</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" t="s">
         <v>60</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" t="s">
         <v>61</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" t="s">
         <v>62</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" t="s">
         <v>63</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" t="s">
         <v>64</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" t="s">
         <v>65</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" t="s">
         <v>66</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" t="s">
         <v>67</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" t="s">
         <v>68</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" t="s">
         <v>69</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" t="s">
         <v>70</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" t="s">
         <v>71</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" t="s">
         <v>72</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" t="s">
         <v>73</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" t="s">
         <v>74</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" t="s">
         <v>75</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" t="s">
         <v>76</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BN1" t="s">
         <v>77</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BO1" t="s">
         <v>78</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BP1" t="s">
         <v>79</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BQ1" t="s">
         <v>80</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BR1" t="s">
         <v>81</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BS1" t="s">
         <v>82</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BT1" t="s">
         <v>83</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BU1" t="s">
         <v>84</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BV1" t="s">
         <v>85</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BW1" t="s">
         <v>86</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BX1" t="s">
         <v>87</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BY1" t="s">
         <v>88</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="BZ1" t="s">
         <v>89</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CA1" t="s">
         <v>90</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CB1" t="s">
         <v>91</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CC1" t="s">
         <v>92</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CD1" t="s">
         <v>93</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CE1" t="s">
         <v>94</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CF1" t="s">
         <v>95</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CG1" t="s">
         <v>96</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CH1" t="s">
         <v>97</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CI1" t="s">
         <v>98</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CJ1" t="s">
         <v>99</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CK1" t="s">
         <v>100</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CL1" t="s">
         <v>101</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CM1" t="s">
         <v>102</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CN1" t="s">
         <v>103</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CO1" t="s">
         <v>104</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CP1" t="s">
         <v>105</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CQ1" t="s">
         <v>106</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CR1" t="s">
         <v>107</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CS1" t="s">
         <v>108</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CT1" t="s">
         <v>109</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CU1" t="s">
         <v>110</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CV1" t="s">
         <v>111</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CW1" t="s">
         <v>112</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CX1" t="s">
         <v>113</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CY1" t="s">
         <v>114</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="CZ1" t="s">
         <v>115</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DA1" t="s">
         <v>116</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DB1" t="s">
         <v>117</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DC1" t="s">
         <v>118</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DD1" t="s">
         <v>119</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DE1" t="s">
         <v>120</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DF1" t="s">
         <v>121</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DG1" t="s">
         <v>122</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DH1" t="s">
         <v>123</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DI1" t="s">
         <v>124</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DJ1" t="s">
         <v>125</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DK1" t="s">
         <v>126</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DL1" t="s">
         <v>127</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DM1" t="s">
         <v>128</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DN1" t="s">
         <v>129</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DO1" t="s">
         <v>130</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DP1" t="s">
         <v>131</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DQ1" t="s">
         <v>132</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DR1" t="s">
         <v>133</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DS1" t="s">
         <v>134</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DT1" t="s">
         <v>135</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DU1" t="s">
         <v>136</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DV1" t="s">
         <v>137</v>
       </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DW1" t="s">
         <v>138</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DX1" t="s">
         <v>139</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DY1" t="s">
         <v>140</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="DZ1" t="s">
         <v>141</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EA1" t="s">
         <v>142</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="EB1" t="s">
         <v>143</v>
       </c>
-      <c r="EC1" s="1" t="s">
+      <c r="EC1" t="s">
         <v>144</v>
       </c>
-      <c r="ED1" s="1" t="s">
+      <c r="ED1" t="s">
         <v>145</v>
       </c>
-      <c r="EE1" s="1" t="s">
+      <c r="EE1" t="s">
         <v>146</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EF1" t="s">
         <v>147</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="EG1" t="s">
         <v>148</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="EH1" t="s">
         <v>149</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EI1" t="s">
         <v>150</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EJ1" t="s">
         <v>151</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EK1" t="s">
         <v>152</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EL1" t="s">
         <v>153</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="EM1" t="s">
         <v>154</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EN1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4238,278 +4192,287 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:144" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>2.8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>5.6</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.35</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
         <v>-53</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
         <v>-34</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
         <v>-19</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>-72</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>-19</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>-61</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>-19</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
         <v>-53</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
         <v>-42</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
         <v>-53</v>
       </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1">
         <v>-53</v>
       </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
+      <c r="X11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1">
         <v>-19</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="1">
         <v>-104</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="1">
         <v>-19</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="1">
         <v>-72</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="1">
         <v>-19</v>
       </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
         <v>-85</v>
       </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
+      <c r="AF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1">
         <v>-53</v>
       </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AS11">
+      <c r="AH11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="1">
         <v>-34</v>
       </c>
-      <c r="AT11">
+      <c r="AT11" s="1">
         <v>-119</v>
       </c>
-      <c r="AU11">
+      <c r="AU11" s="1">
         <v>-34</v>
       </c>
-      <c r="AV11">
+      <c r="AV11" s="1">
         <v>-101</v>
       </c>
-      <c r="AW11">
+      <c r="AW11" s="1">
         <v>-34</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="1">
         <v>-19</v>
       </c>
-      <c r="AY11">
+      <c r="AY11" s="1">
         <v>-104</v>
       </c>
-      <c r="AZ11">
+      <c r="AZ11" s="1">
         <v>-19</v>
       </c>
-      <c r="BA11">
+      <c r="BA11" s="1">
         <v>-86</v>
       </c>
-      <c r="BB11">
+      <c r="BB11" s="1">
         <v>-19</v>
       </c>
-      <c r="BC11">
-        <v>0</v>
-      </c>
-      <c r="BD11">
+      <c r="BC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="1">
         <v>-85</v>
       </c>
-      <c r="BE11">
-        <v>0</v>
-      </c>
-      <c r="BF11">
+      <c r="BE11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF11" s="1">
         <v>-67</v>
       </c>
-      <c r="BG11">
-        <v>0</v>
-      </c>
-      <c r="BM11">
+      <c r="BG11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM11" s="1">
         <v>-19</v>
       </c>
-      <c r="BN11">
+      <c r="BN11" s="1">
         <v>-104</v>
       </c>
-      <c r="BO11">
+      <c r="BO11" s="1">
         <v>-19</v>
       </c>
-      <c r="BP11">
+      <c r="BP11" s="1">
         <v>-104</v>
       </c>
-      <c r="BQ11">
+      <c r="BQ11" s="1">
         <v>-19</v>
       </c>
-      <c r="BR11">
-        <v>0</v>
-      </c>
-      <c r="BS11">
+      <c r="BR11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS11" s="1">
         <v>-85</v>
       </c>
-      <c r="BT11">
-        <v>0</v>
-      </c>
-      <c r="BU11">
+      <c r="BT11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU11" s="1">
         <v>-85</v>
       </c>
-      <c r="BV11">
-        <v>0</v>
-      </c>
-      <c r="CH11">
+      <c r="BV11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH11" s="1">
         <v>-85</v>
       </c>
-      <c r="CJ11">
+      <c r="CI11">
+        <v>0</v>
+      </c>
+      <c r="CJ11" s="1">
         <v>-106</v>
       </c>
-      <c r="CQ11">
-        <v>0</v>
-      </c>
-      <c r="CR11">
+      <c r="CK11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR11" s="1">
         <v>56</v>
       </c>
-      <c r="CS11">
-        <v>0</v>
-      </c>
-      <c r="CT11">
+      <c r="CS11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT11" s="1">
         <v>63</v>
       </c>
-      <c r="CU11">
-        <v>0</v>
-      </c>
-      <c r="CV11">
-        <v>0</v>
-      </c>
-      <c r="CW11">
+      <c r="CU11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW11" s="1">
         <v>56</v>
       </c>
-      <c r="CX11">
-        <v>0</v>
-      </c>
-      <c r="CY11">
+      <c r="CX11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY11" s="1">
         <v>80</v>
       </c>
-      <c r="CZ11">
-        <v>0</v>
-      </c>
-      <c r="DA11">
+      <c r="CZ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA11" s="1">
         <v>19</v>
       </c>
-      <c r="DB11">
+      <c r="DB11" s="1">
         <v>90</v>
       </c>
-      <c r="DC11">
+      <c r="DC11" s="1">
         <v>19</v>
       </c>
-      <c r="DD11">
+      <c r="DD11" s="1">
         <v>99</v>
       </c>
-      <c r="DE11">
+      <c r="DE11" s="1">
         <v>19</v>
       </c>
-      <c r="DF11">
-        <v>0</v>
-      </c>
-      <c r="DG11">
+      <c r="DF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG11" s="1">
         <v>71</v>
       </c>
-      <c r="DH11">
-        <v>0</v>
-      </c>
-      <c r="DI11">
+      <c r="DH11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI11" s="1">
         <v>80</v>
       </c>
-      <c r="DJ11">
-        <v>0</v>
-      </c>
-      <c r="DK11">
+      <c r="DJ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK11" s="1">
         <v>19</v>
       </c>
-      <c r="DL11">
+      <c r="DL11" s="1">
         <v>109</v>
       </c>
-      <c r="DM11">
+      <c r="DM11" s="1">
         <v>19</v>
       </c>
-      <c r="DN11">
+      <c r="DN11" s="1">
         <v>119</v>
       </c>
-      <c r="DO11">
+      <c r="DO11" s="1">
         <v>19</v>
       </c>
-      <c r="DP11">
-        <v>0</v>
-      </c>
-      <c r="DQ11">
+      <c r="DP11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ11" s="1">
         <v>90</v>
       </c>
-      <c r="DR11">
-        <v>0</v>
-      </c>
-      <c r="DS11">
+      <c r="DR11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS11" s="1">
         <v>100</v>
       </c>
-      <c r="DT11">
+      <c r="DT11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -16328,9 +16291,6 @@
         <v>-150</v>
       </c>
       <c r="BV43">
-        <v>0</v>
-      </c>
-      <c r="CI43">
         <v>0</v>
       </c>
       <c r="CQ43">

</xml_diff>